<commit_message>
initalization of adding classroms to subjects
</commit_message>
<xml_diff>
--- a/data/testdata/SSG_CLASSROOMS.xlsx
+++ b/data/testdata/SSG_CLASSROOMS.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">classroom_name</t>
   </si>
   <si>
-    <t xml:space="preserve">type</t>
+    <t xml:space="preserve">type_id</t>
   </si>
 </sst>
 </file>
@@ -131,15 +131,15 @@
   </sheetPr>
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>